<commit_message>
Dodana nova tabela, ureditev tabel, popravitel tabel, nemorm spremenit legende v tabeli za slovenijo
</commit_message>
<xml_diff>
--- a/podatki/Pregled_pridelkov_regije.xlsx
+++ b/podatki/Pregled_pridelkov_regije.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakab\Desktop\R-Projekt-Naloga\APPR-2020-21\podatki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C312606D-8372-404A-9855-9F296169F92A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178A3364-2660-451D-9AFF-0149B51C66BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="2565" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
     <t>leto</t>
   </si>
   <si>
-    <t>Slovenska_regija</t>
+    <t>Regija</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
dodajanje opisa in grafov v rmd
</commit_message>
<xml_diff>
--- a/podatki/Pregled_pridelkov_regije.xlsx
+++ b/podatki/Pregled_pridelkov_regije.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakab\Desktop\R-Projekt-Naloga\APPR-2020-21\podatki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C312606D-8372-404A-9855-9F296169F92A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178A3364-2660-451D-9AFF-0149B51C66BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="2565" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
     <t>leto</t>
   </si>
   <si>
-    <t>Slovenska_regija</t>
+    <t>Regija</t>
   </si>
 </sst>
 </file>

</xml_diff>